<commit_message>
20171222 修正Google Excel問題單 第96 97 98 100條
</commit_message>
<xml_diff>
--- a/templates/班機表欄位.xlsx
+++ b/templates/班機表欄位.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\case\20170116_Module\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EWS\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -390,6 +390,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -455,20 +469,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
         </patternFill>
       </fill>
     </dxf>
@@ -817,7 +817,7 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="I12" sqref="I11:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1041,44 +1041,47 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="D4">
-    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="13" stopIfTrue="1">
       <formula>AND(COUNTIF($C$5:$C$62731,D4)+COUNTIF($C$1:$C$4,D4)&gt;1,NOT(ISBLANK(D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C4000">
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="10" priority="5">
       <formula>$C5="移倉"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="9" priority="6">
       <formula>$C5="X3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="8" priority="7">
       <formula>$C5="G1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>LENB($C5)&gt;5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:I5 A6:XFD4000 K5:XFD5">
-    <cfRule type="expression" dxfId="4" priority="13">
+    <cfRule type="expression" dxfId="6" priority="14">
       <formula>$B5="特特貨"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="14">
+    <cfRule type="expression" dxfId="5" priority="15">
       <formula>$B5="普特貨"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F4000">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>VALUE($F5)&gt;70</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$B5="特特貨"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$B5="普特貨"</formula>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>